<commit_message>
with linest fit in excel
</commit_message>
<xml_diff>
--- a/Experiments/Rolling_motion/Final.xlsx
+++ b/Experiments/Rolling_motion/Final.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>下落高度h(m)</t>
   </si>
@@ -107,12 +107,39 @@
   <si>
     <t>Vx^2</t>
   </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>slope err</t>
+  </si>
+  <si>
+    <t>r^2</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Reg SS</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Intercept error</t>
+  </si>
+  <si>
+    <t>std error on y</t>
+  </si>
+  <si>
+    <t>Deg of freedom</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +161,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -159,7 +194,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -179,6 +214,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -197,6 +235,1199 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10587270341207349"/>
+          <c:y val="0.11615740740740743"/>
+          <c:w val="0.86164129483814522"/>
+          <c:h val="0.83291666666666664"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet2!$R$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>4.3046946586199547E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet2!$R$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>4.3046946586199547E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$N$2:$N$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>4.1459708311584553E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8840551215052203E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4023936700616677E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7766760937373118E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5286480877065666E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1683447473078009E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3279080311204686E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7500387987497024E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2165983054484303E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6475035909530029E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0760790730661975E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.935482591466196E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.638430000343146E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.537158561492634E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.721921441756927E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.0815181516332884E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.5129054290117278E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.9846870192453234E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.3101699244583327E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.10274479016340386</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.11444825078196491</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.11722178552979558</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.13587610855842552</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.14970698471744126</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.16153784102978225</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.17234066837754874</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.18096895662983303</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.1963036659307224</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.22415377928862706</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.23041717164793762</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.25013772706352083</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.26780824496621525</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.28616530470984769</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.31497844817953868</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.3144977712467773</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.3297373380947517</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.33497602948728966</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$O$2:$O$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1.262658453882196E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1414946750269079E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.281211012428037E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4208673983253726E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4952871151909995E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9603766253314361E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1521938480655368E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4319296435142963E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7673949405551204E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1242972774212594E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5240736918453353E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.9399250531536069E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4466286716885509E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.941489183994942E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.5409295288020611E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.147191168741445E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.7784615515627698E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.421859571688531E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.0925427688555281E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.7624564725947472E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.5831841190101964E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.3357068291218346E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.017538341006668E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1049919930760526E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.1974727786606723E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.2919010715185534E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.3905304863737349E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.4897325063119865E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5965732968007459E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7099066382976966E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.8198023305438762E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.9424922571429803E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.0604630613317961E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.1912644011424731E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.3214589579882039E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.4520610733098677E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.5884995753694493E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-850D-4610-A822-16BBC467C03A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="561533984"/>
+        <c:axId val="561538904"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="561533984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561538904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="561538904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561533984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>252411</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,10 +1714,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
@@ -960,10 +2191,10 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="8"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1719,10 +2950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N122"/>
+  <dimension ref="A1:S122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1735,9 +2966,12 @@
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1">
+    <row r="1" spans="1:19" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +3009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1.1924999999999999</v>
       </c>
@@ -1818,8 +3052,24 @@
         <f>ABS(F2)^2</f>
         <v>4.1459708311584553E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2">
+        <v>1.262658453882196E-4</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2">
+        <f t="array" ref="Q2:R6">LINEST(M2:M38,N2:N38,FALSE,TRUE)</f>
+        <v>7.3902359919299207E-2</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1.1924999999999999</v>
       </c>
@@ -1862,8 +3112,23 @@
         <f t="shared" ref="N3:N12" si="5">ABS(F3)^2</f>
         <v>1.8840551215052203E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3">
+        <v>2.1414946750269079E-4</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3">
+        <v>4.3439000992437577E-4</v>
+      </c>
+      <c r="R3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1.1924999999999999</v>
       </c>
@@ -1906,8 +3171,23 @@
         <f t="shared" si="5"/>
         <v>2.4023936700616677E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4">
+        <v>3.281211012428037E-4</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4">
+        <v>0.99875775942334399</v>
+      </c>
+      <c r="R4">
+        <v>4.3046946586199547E-4</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1.1924999999999999</v>
       </c>
@@ -1950,8 +3230,23 @@
         <f t="shared" si="5"/>
         <v>4.7766760937373118E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5">
+        <v>4.4208673983253726E-4</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5">
+        <v>28943.893811639398</v>
+      </c>
+      <c r="R5">
+        <v>36</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1.1924999999999999</v>
       </c>
@@ -1994,8 +3289,23 @@
         <f t="shared" si="5"/>
         <v>9.5286480877065666E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6">
+        <v>6.4952871151909995E-4</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6">
+        <v>5.3634181712037899E-3</v>
+      </c>
+      <c r="R6">
+        <v>6.6709425974224206E-6</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1.1924999999999999</v>
       </c>
@@ -2038,8 +3348,11 @@
         <f t="shared" si="5"/>
         <v>1.1683447473078009E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7">
+        <v>8.9603766253314361E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1.1924999999999999</v>
       </c>
@@ -2082,8 +3395,11 @@
         <f t="shared" si="5"/>
         <v>1.3279080311204686E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8">
+        <v>1.1521938480655368E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>1.1924999999999999</v>
       </c>
@@ -2126,8 +3442,11 @@
         <f t="shared" si="5"/>
         <v>1.7500387987497024E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9">
+        <v>1.4319296435142963E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1.1924999999999999</v>
       </c>
@@ -2170,8 +3489,11 @@
         <f t="shared" si="5"/>
         <v>2.2165983054484303E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10">
+        <v>1.7673949405551204E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>1.1924999999999999</v>
       </c>
@@ -2214,8 +3536,11 @@
         <f t="shared" si="5"/>
         <v>2.6475035909530029E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11">
+        <v>2.1242972774212594E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1.1924999999999999</v>
       </c>
@@ -2258,8 +3583,11 @@
         <f t="shared" si="5"/>
         <v>3.0760790730661975E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12">
+        <v>2.5240736918453353E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>1.1924999999999999</v>
       </c>
@@ -2302,8 +3630,11 @@
         <f t="shared" ref="N13:N76" si="7">ABS(F13)^2</f>
         <v>3.935482591466196E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13">
+        <v>2.9399250531536069E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>1.1924999999999999</v>
       </c>
@@ -2346,8 +3677,11 @@
         <f t="shared" si="7"/>
         <v>4.638430000343146E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14">
+        <v>3.4466286716885509E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>1.1924999999999999</v>
       </c>
@@ -2390,8 +3724,11 @@
         <f t="shared" si="7"/>
         <v>5.537158561492634E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15">
+        <v>3.941489183994942E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>1.1924999999999999</v>
       </c>
@@ -2434,8 +3771,11 @@
         <f t="shared" si="7"/>
         <v>6.721921441756927E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16">
+        <v>4.5409295288020611E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>1.1924999999999999</v>
       </c>
@@ -2478,8 +3818,13 @@
         <f t="shared" si="7"/>
         <v>7.0815181516332884E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17">
+        <v>5.147191168741445E-3</v>
+      </c>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>1.1924999999999999</v>
       </c>
@@ -2522,8 +3867,11 @@
         <f t="shared" si="7"/>
         <v>7.5129054290117278E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="O18">
+        <v>5.7784615515627698E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>1.1924999999999999</v>
       </c>
@@ -2566,8 +3914,11 @@
         <f t="shared" si="7"/>
         <v>7.9846870192453234E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19">
+        <v>6.421859571688531E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>1.1924999999999999</v>
       </c>
@@ -2610,8 +3961,11 @@
         <f t="shared" si="7"/>
         <v>8.3101699244583327E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20">
+        <v>7.0925427688555281E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>1.1924999999999999</v>
       </c>
@@ -2654,8 +4008,11 @@
         <f t="shared" si="7"/>
         <v>0.10274479016340386</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="O21">
+        <v>7.7624564725947472E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>1.1924999999999999</v>
       </c>
@@ -2698,8 +4055,11 @@
         <f t="shared" si="7"/>
         <v>0.11444825078196491</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="O22">
+        <v>8.5831841190101964E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>1.1924999999999999</v>
       </c>
@@ -2742,8 +4102,11 @@
         <f t="shared" si="7"/>
         <v>0.11722178552979558</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="O23">
+        <v>9.3357068291218346E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>1.1924999999999999</v>
       </c>
@@ -2786,8 +4149,11 @@
         <f t="shared" si="7"/>
         <v>0.13587610855842552</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="O24">
+        <v>1.017538341006668E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25">
         <v>1.1924999999999999</v>
       </c>
@@ -2830,8 +4196,11 @@
         <f t="shared" si="7"/>
         <v>0.14970698471744126</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25">
+        <v>1.1049919930760526E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26">
         <v>1.1924999999999999</v>
       </c>
@@ -2874,8 +4243,11 @@
         <f t="shared" si="7"/>
         <v>0.16153784102978225</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="O26">
+        <v>1.1974727786606723E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>1.1924999999999999</v>
       </c>
@@ -2918,8 +4290,11 @@
         <f t="shared" si="7"/>
         <v>0.17234066837754874</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="O27">
+        <v>1.2919010715185534E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>1.1924999999999999</v>
       </c>
@@ -2962,8 +4337,11 @@
         <f t="shared" si="7"/>
         <v>0.18096895662983303</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="O28">
+        <v>1.3905304863737349E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>1.1924999999999999</v>
       </c>
@@ -3006,8 +4384,11 @@
         <f t="shared" si="7"/>
         <v>0.1963036659307224</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29">
+        <v>1.4897325063119865E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30">
         <v>1.1924999999999999</v>
       </c>
@@ -3050,8 +4431,11 @@
         <f t="shared" si="7"/>
         <v>0.22415377928862706</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="O30">
+        <v>1.5965732968007459E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31">
         <v>1.1924999999999999</v>
       </c>
@@ -3094,8 +4478,11 @@
         <f t="shared" si="7"/>
         <v>0.23041717164793762</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="O31">
+        <v>1.7099066382976966E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32">
         <v>1.1924999999999999</v>
       </c>
@@ -3138,8 +4525,11 @@
         <f t="shared" si="7"/>
         <v>0.25013772706352083</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="O32">
+        <v>1.8198023305438762E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33">
         <v>1.1924999999999999</v>
       </c>
@@ -3182,8 +4572,11 @@
         <f t="shared" si="7"/>
         <v>0.26780824496621525</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="O33">
+        <v>1.9424922571429803E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34">
         <v>1.1924999999999999</v>
       </c>
@@ -3226,8 +4619,11 @@
         <f t="shared" si="7"/>
         <v>0.28616530470984769</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="O34">
+        <v>2.0604630613317961E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35">
         <v>1.1924999999999999</v>
       </c>
@@ -3270,8 +4666,11 @@
         <f t="shared" si="7"/>
         <v>0.31497844817953868</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="O35">
+        <v>2.1912644011424731E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36">
         <v>1.1924999999999999</v>
       </c>
@@ -3314,8 +4713,11 @@
         <f t="shared" si="7"/>
         <v>0.3144977712467773</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="O36">
+        <v>2.3214589579882039E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37">
         <v>1.1924999999999999</v>
       </c>
@@ -3358,8 +4760,11 @@
         <f t="shared" si="7"/>
         <v>0.3297373380947517</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="O37">
+        <v>2.4520610733098677E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38">
         <v>1.1924999999999999</v>
       </c>
@@ -3402,8 +4807,11 @@
         <f t="shared" si="7"/>
         <v>0.33497602948728966</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="O38">
+        <v>2.5884995753694493E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="2"/>
@@ -3411,7 +4819,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" s="5" customFormat="1">
+    <row r="40" spans="1:15" s="5" customFormat="1">
       <c r="A40" s="5" t="s">
         <v>16</v>
       </c>
@@ -3445,7 +4853,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="A41" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -3489,7 +4897,7 @@
         <v>3.8651830718674032E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:15">
       <c r="A42" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -3533,7 +4941,7 @@
         <v>5.1273604694240295E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:15">
       <c r="A43" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -3577,7 +4985,7 @@
         <v>8.524666741053801E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:15">
       <c r="A44" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -3621,7 +5029,7 @@
         <v>1.4872222761029888E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:15">
       <c r="A45" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -3665,7 +5073,7 @@
         <v>2.8062587384956573E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:15">
       <c r="A46" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -3709,7 +5117,7 @@
         <v>7.0661183269098678E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:15">
       <c r="A47" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -3753,7 +5161,7 @@
         <v>9.8456869707843116E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:15">
       <c r="A48" s="4">
         <v>1.0449999999999999</v>
       </c>
@@ -7010,6 +8418,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
with modification on angle
</commit_message>
<xml_diff>
--- a/Experiments/Rolling_motion/Final.xlsx
+++ b/Experiments/Rolling_motion/Final.xlsx
@@ -1399,16 +1399,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>252411</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>23811</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2953,7 +2953,7 @@
   <dimension ref="A1:S122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4199,6 +4199,10 @@
       <c r="O25">
         <v>1.1049919930760526E-2</v>
       </c>
+      <c r="Q25">
+        <f>(Q2*A2*9.8-0.5*A2)*2*B2^2</f>
+        <v>1.3910664516822221E-3</v>
+      </c>
     </row>
     <row r="26" spans="1:18">
       <c r="A26">

</xml_diff>